<commit_message>
add libs and new apk
</commit_message>
<xml_diff>
--- a/AgroComplit/наименования.xlsx
+++ b/AgroComplit/наименования.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
   <si>
     <t>Зерновые</t>
   </si>
@@ -261,31 +261,7 @@
     <t>Разное</t>
   </si>
   <si>
-    <t>итого денег за день</t>
-  </si>
-  <si>
-    <t>выборка по дням</t>
-  </si>
-  <si>
-    <t>правильно считать сумму</t>
-  </si>
-  <si>
-    <t>скидка</t>
-  </si>
-  <si>
     <t>Продукты</t>
-  </si>
-  <si>
-    <t>добавить новые группы</t>
-  </si>
-  <si>
-    <t>где то выбивает новое окно</t>
-  </si>
-  <si>
-    <t>сервер</t>
-  </si>
-  <si>
-    <t>разобраться с кг или мешок</t>
   </si>
 </sst>
 </file>
@@ -335,7 +311,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,12 +327,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -456,9 +426,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -744,7 +711,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,7 +974,7 @@
     </row>
     <row r="13" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>79</v>
@@ -1035,9 +1002,7 @@
       <c r="B15" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>80</v>
-      </c>
+      <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
@@ -1048,9 +1013,7 @@
       <c r="B16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>81</v>
-      </c>
+      <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
@@ -1061,9 +1024,7 @@
       <c r="B17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>82</v>
-      </c>
+      <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1073,9 +1034,7 @@
       <c r="B18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>83</v>
-      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1083,9 +1042,7 @@
       <c r="B19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>85</v>
-      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="G19" s="5"/>
     </row>
@@ -1094,9 +1051,7 @@
       <c r="B20" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>86</v>
-      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
     </row>
@@ -1105,9 +1060,7 @@
       <c r="B21" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>87</v>
-      </c>
+      <c r="D21" s="9"/>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
     </row>
@@ -1116,9 +1069,7 @@
       <c r="B22" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>88</v>
-      </c>
+      <c r="D22" s="9"/>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
     </row>

</xml_diff>